<commit_message>
adding lektion 1 to csv
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Nouns" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="old" sheetId="5" state="hidden" r:id="rId6"/>
     <sheet name="old_comprehension" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="Comprehension" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Lessons" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7392" uniqueCount="3992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7545" uniqueCount="4089">
   <si>
     <t xml:space="preserve">German</t>
   </si>
@@ -12020,6 +12021,339 @@
   <si>
     <t xml:space="preserve">Es ist ___, bei Fieber zu Hause zu bleiben.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Frage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lektion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Ananas rot?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist gelb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lektion-0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Brokkoli grün?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, er ist grün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist gelb und krumm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist das Wetter heute?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist sonnig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Apfel ist rot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist grün zwischen Apfel, Karotte?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Apfel ist grün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Tomate blau?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist rot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Kürbis?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist orange und rund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Zitrone süß?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist sauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Himmel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist blau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist grün und frisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Aubergine lila?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, sie ist lila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist gelb zwischen Zitrone, Himbeere, Tomate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Zitrone ist gelb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist das Wetter warm im Winter?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, es ist kalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Apfel, rot oder orange?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist rot</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wie ist der Schnee, warm und </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">weiß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, oder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">weiß und kalt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">?</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist weiß und kalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Möhre lila?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist lila?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Aubergine ist lila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist das Wetter sonnig im Regen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, es ist nass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist die Gurke, kurz oder lang?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist lang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Himmel grün?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, er ist blau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist das Wetter im Sommer, warm und sonnig, oder kalt?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist warm und sonnig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Spinat gelb?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, er ist grün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist die Tomate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist rot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Apfel blau?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, er ist rot oder grün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist die Himbeere?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist rot und klein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Kürbis blau?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, er ist orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist rund und gelb?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Zitrone ist rund und gelb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist das Wetter im Herbst?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist kühl und windig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist rot zwischen Apfel, Gurke und Zwiebel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Paprika rot?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, sie kann rot sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Brokkoli?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist grün und buschig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Erdbeere lila?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist kalt zwischen Tee, Eis, Suppe?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Eis ist kalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Regen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist nass und kühl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Mais blau?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, er ist gelb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist orange zwischen Möhre, Apfel, Banane?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Möhre ist orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist die Zwiebel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist rund und weiß</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Banane grün?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchmal, wenn sie nicht reif ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist kühl?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Wind ist kühl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist die Orange?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie ist rund und orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Kartoffel blau?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist braun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist gelb und krumm?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Banane ist gelb und krumm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Wind?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist stark oder schwach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist die Zucchini rosa?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein, sie ist grün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was ist rund zwischen Kürbis, Möhre, Gurke?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Kürbis ist rund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Himmel im Sommer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist blau und klar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Spinat rot?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wie ist der Nebel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er ist grau und dick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Himmel gelb?</t>
+  </si>
 </sst>
 </file>
 
@@ -12028,7 +12362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -12069,6 +12403,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -12162,10 +12501,10 @@
   <dimension ref="A1:E556"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
@@ -18283,7 +18622,7 @@
       <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.1"/>
@@ -19200,11 +19539,11 @@
   </sheetPr>
   <dimension ref="A1:D1162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A449" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1173" activeCellId="0" sqref="A1173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.07"/>
@@ -32056,7 +32395,7 @@
       <selection pane="topLeft" activeCell="A204" activeCellId="0" sqref="A204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.62"/>
   </cols>
@@ -33588,7 +33927,7 @@
       <selection pane="topLeft" activeCell="D348" activeCellId="0" sqref="D348"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
@@ -38712,7 +39051,7 @@
       <selection pane="topLeft" activeCell="B167" activeCellId="0" sqref="B167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
@@ -41021,11 +41360,11 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
   </cols>
@@ -41239,6 +41578,595 @@
       </c>
       <c r="C19" s="0" t="s">
         <v>3957</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>3992</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3993</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3995</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3996</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3998</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3999</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3537</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4000</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4001</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>4002</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3532</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4003</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4004</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>4005</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4006</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>4007</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4008</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4009</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>4011</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4012</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4013</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>3556</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>4014</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>4015</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>4016</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>4018</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4019</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4021</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>4022</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4023</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>4024</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4025</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>4026</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>4027</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4029</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>4030</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4031</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>4032</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>4033</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>4034</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>4035</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>4036</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>4037</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>4038</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>4040</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>4042</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>4045</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>4047</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>4048</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>4049</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>4050</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>4051</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>4003</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>4053</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>4007</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>4058</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>4059</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>4060</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>4062</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>4063</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>4064</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>4065</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>4066</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>4067</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>4068</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>4070</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>4071</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>4072</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>4073</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>4074</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>4075</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>4076</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>4077</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>4078</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>4079</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>4080</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>4081</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>4082</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>4083</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>4084</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>4085</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>4038</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>4086</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>4087</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>4088</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>4034</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>3997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>